<commit_message>
Wrote Permis, did compare
</commit_message>
<xml_diff>
--- a/Dokumentation/lni/images/Vergleich.xlsx
+++ b/Dokumentation/lni/images/Vergleich.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRV-WIN-10\Documents\swe-security\swe-security\Dokumentation\lni\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\swe-security\Dokumentation\lni\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86995F19-AF2F-4935-9BC5-CEA9007A3C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7988FA-FF3A-4C29-BC9F-9B715E8BE9F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D0863FCA-48D3-438B-815E-72DC6B1A5B07}"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" xr2:uid="{D0863FCA-48D3-438B-815E-72DC6B1A5B07}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Vergleich der Sicherheitskonzepte</t>
   </si>
@@ -108,6 +108,63 @@
   </si>
   <si>
     <t>Authentifizierung nur bei speziellen Anwendungsfällen relevant.</t>
+  </si>
+  <si>
+    <t>Permis</t>
+  </si>
+  <si>
+    <t>Vertraulichkeit der Daten wird durch Verwendung der asymmetrischen Kryptographie geschützt</t>
+  </si>
+  <si>
+    <t>Integrität der Daten wird durch Verwendung der asymmetrischen Kryptographie geschützt</t>
+  </si>
+  <si>
+    <t>Authetifizierung erfolgt über die die Zertifikate</t>
+  </si>
+  <si>
+    <t>Erfolgt über die Access Controll Lists</t>
+  </si>
+  <si>
+    <t>Nicht-Anfechtbarkeit ist über die Public-Key-Infrastructure gegeben.</t>
+  </si>
+  <si>
+    <t>Ein Benutzer kann über das Proxy-Zertifikat authetifiziert werden</t>
+  </si>
+  <si>
+    <t>Autorisierung erfolgt über die Richtlinien der Webseite und Gemeinschaft. Die Infromationen befinden sich im Proxy-Zertifikat</t>
+  </si>
+  <si>
+    <t>Nicht-Anfechtbarkeit ist über Proxy-Zertifikat gegeben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorisierung erfolgt über den Server und die dort definierten Autorisierungsrichtlinien </t>
+  </si>
+  <si>
+    <t>Erfolgt über Distinguished Name des Attribut-Zertifikats.</t>
+  </si>
+  <si>
+    <t>Keine näheren Infromationen</t>
+  </si>
+  <si>
+    <t>Vertraulichkeit wird mit den Attribut Zertifikaten geschützt</t>
+  </si>
+  <si>
+    <t>Datenintegriät ist über das Proxy-Zertifikat gegeben</t>
+  </si>
+  <si>
+    <t>Integrität ist über Attribut Zertifikat gegeben</t>
+  </si>
+  <si>
+    <t>Nicht-Anfechtbarkeit ist über Attribut Zertifikat gegeben</t>
+  </si>
+  <si>
+    <t>Werden nach Authentifizierung über Proxy-Zertifikat geschützt. Anfragen erfolgen nur über die Proxy Credentials.</t>
+  </si>
+  <si>
+    <t>Server, der alle Attribut-Zertifikate hostet muss zusätzlich geschützt werden. Fällt er aus, funktioniert das System nicht.</t>
+  </si>
+  <si>
+    <t>CAS Serve muss zusätzlich geschützt werden. Fällt er aus, funktioniert das System nicht.</t>
   </si>
 </sst>
 </file>
@@ -137,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +248,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -389,6 +452,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -402,15 +480,21 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -447,56 +531,50 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -819,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388784D2-EFFD-4DC5-9F65-4D4C139335CC}">
-  <dimension ref="B2:G36"/>
+  <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,335 +908,413 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="6" width="30.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D4" s="33" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="29" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="30"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="3"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="H6" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="F12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="33"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="33"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="33"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="33"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="11" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="21"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="21"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="22"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="F17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="33"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="33"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="33"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="33"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="11" t="s">
+      <c r="C22" s="8"/>
+      <c r="D22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="20"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="21"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="21"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="22"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="s">
+      <c r="F22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="33"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="33"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="33"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="33"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="21"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="21"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="21"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="22"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+      <c r="F27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="33"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="33"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="33"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="23"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="33"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="11" t="s">
+      <c r="C32" s="8"/>
+      <c r="D32" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="21"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="21"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="21"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="22"/>
+      <c r="F32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="33"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="33"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="33"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="D4:E5"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="B7:C11"/>
-    <mergeCell ref="B12:C16"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="F12:F16"/>
+  <mergeCells count="38">
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="H32:H36"/>
+    <mergeCell ref="F4:H5"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="H12:H16"/>
+    <mergeCell ref="B27:C31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="B32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="G32:G36"/>
     <mergeCell ref="G7:G11"/>
     <mergeCell ref="G12:G16"/>
-    <mergeCell ref="F4:G5"/>
     <mergeCell ref="B22:C26"/>
     <mergeCell ref="D22:D26"/>
     <mergeCell ref="E22:E26"/>
@@ -1169,16 +1325,15 @@
     <mergeCell ref="E17:E21"/>
     <mergeCell ref="F17:F21"/>
     <mergeCell ref="G17:G21"/>
-    <mergeCell ref="B32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="G32:G36"/>
-    <mergeCell ref="B27:C31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="B7:C11"/>
+    <mergeCell ref="B12:C16"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="F12:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>